<commit_message>
% de aprobación de los recuperatorios
</commit_message>
<xml_diff>
--- a/Planilla Notas General 2023 2do Semestre.xlsx
+++ b/Planilla Notas General 2023 2do Semestre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCRITORIO\GESTION-DE-LA-CALIDAD-Y-MEJORA-CONTINUA\TP 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE53E7A1-42A0-4832-8FB1-322A42B16487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390A860A-8AAE-49BD-9C2C-210721B7A8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCA0D012-0B3A-4387-9D5C-6147A5A80283}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="152">
   <si>
     <t>aus</t>
   </si>
@@ -447,13 +447,40 @@
     <t>Sofie Shenniel</t>
   </si>
   <si>
-    <t>N° Aprobados</t>
-  </si>
-  <si>
-    <t>N° Desaprobados</t>
-  </si>
-  <si>
-    <t>% aprobados</t>
+    <t>N° Aprobados FINAL</t>
+  </si>
+  <si>
+    <t>% aprobados FINAL</t>
+  </si>
+  <si>
+    <t>N° Desaprobados FINAL</t>
+  </si>
+  <si>
+    <t>N° Aprobados RE1</t>
+  </si>
+  <si>
+    <t>N° Desaprobados RE1</t>
+  </si>
+  <si>
+    <t>% aprobados RE1</t>
+  </si>
+  <si>
+    <t>N° Aprobados RE2</t>
+  </si>
+  <si>
+    <t>N° Desaprobados RE2</t>
+  </si>
+  <si>
+    <t>% aprobados RE2</t>
+  </si>
+  <si>
+    <t>N° Aprobados RE3</t>
+  </si>
+  <si>
+    <t>N° Desaprobados RE3</t>
+  </si>
+  <si>
+    <t>% aprobados RE3</t>
   </si>
 </sst>
 </file>
@@ -945,7 +972,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +985,7 @@
     <col min="11" max="11" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" style="1"/>
     <col min="13" max="13" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -1000,7 +1027,7 @@
         <v>140</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
@@ -1094,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N4" s="8"/>
     </row>
@@ -1277,7 +1304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1307,8 +1334,14 @@
       <c r="K11" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1340,8 +1373,16 @@
       <c r="K12" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M12" s="7">
+        <f>COUNTIF($E$2:$E$61,"&gt;=60")</f>
+        <v>13</v>
+      </c>
+      <c r="N12" s="7">
+        <f>COUNTIF(E2:E61,"&lt;60")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1365,8 +1406,10 @@
       <c r="K13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1396,8 +1439,12 @@
       <c r="K14" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M14" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1429,6 +1476,11 @@
       <c r="K15" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="M15" s="10">
+        <f>M12/(M12+N12)</f>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1461,7 +1513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1492,7 +1544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -1525,7 +1577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1558,7 +1610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -1592,8 +1644,14 @@
       <c r="K20" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>58</v>
       </c>
@@ -1617,8 +1675,16 @@
       <c r="K21" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21" s="7">
+        <f>COUNTIF($F$2:$F$61,"&gt;=60")</f>
+        <v>8</v>
+      </c>
+      <c r="N21" s="7">
+        <f>COUNTIF(F2:F61,"&lt;60")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
@@ -1642,8 +1708,10 @@
       <c r="K22" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -1675,8 +1743,12 @@
       <c r="K23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -1708,8 +1780,13 @@
       <c r="K24" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24" s="10">
+        <f>M21/(M21+N21)</f>
+        <v>0.5</v>
+      </c>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>66</v>
       </c>
@@ -1742,7 +1819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>68</v>
       </c>
@@ -1777,7 +1854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>71</v>
       </c>
@@ -1810,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>73</v>
       </c>
@@ -1840,8 +1917,14 @@
       <c r="K28" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>75</v>
       </c>
@@ -1869,8 +1952,16 @@
       <c r="K29" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M29" s="7">
+        <f>COUNTIF($H$2:$H$61,"&gt;=60")</f>
+        <v>11</v>
+      </c>
+      <c r="N29" s="7">
+        <f>COUNTIF(H2:H61,"&lt;60")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1898,8 +1989,10 @@
       <c r="K30" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>79</v>
       </c>
@@ -1933,8 +2026,12 @@
       <c r="K31" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M31" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>81</v>
       </c>
@@ -1964,6 +2061,11 @@
       <c r="K32" s="2">
         <v>8</v>
       </c>
+      <c r="M32" s="10">
+        <f>M29/(M29+N29)</f>
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="N32" s="8"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">

</xml_diff>